<commit_message>
all in on blizzard
</commit_message>
<xml_diff>
--- a/investments.xlsx
+++ b/investments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\stock_journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09E94E7-9536-41E2-A9B1-FE9DA43C05B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AFFBAD-2715-4D91-BC3F-99D8DD21B45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="3390" windowWidth="21405" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="4215" windowWidth="21405" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>stock</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>23/11/2021</t>
+  </si>
+  <si>
+    <t>Activision Blizzard</t>
+  </si>
+  <si>
+    <t>ATVI</t>
   </si>
 </sst>
 </file>
@@ -132,11 +138,14 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -164,8 +173,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D1F8B31-3FDA-4128-9E90-787B32745CE5}" name="Table1" displayName="Table1" ref="A1:I12" totalsRowShown="0">
-  <autoFilter ref="A1:I12" xr:uid="{4D1F8B31-3FDA-4128-9E90-787B32745CE5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D1F8B31-3FDA-4128-9E90-787B32745CE5}" name="Table1" displayName="Table1" ref="A1:I11" totalsRowShown="0">
+  <autoFilter ref="A1:I11" xr:uid="{4D1F8B31-3FDA-4128-9E90-787B32745CE5}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{760083B0-21AC-420E-81F7-CAA636D86707}" name="date in" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{75A00969-4119-4764-BE45-739E5B52C708}" name="date out" dataDxfId="0"/>
@@ -444,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,6 +594,23 @@
         <v>1.6446832763393593E-2</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3861.24</v>
+      </c>
+      <c r="F5" s="2">
+        <v>83.94</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>